<commit_message>
Changes in supplementary materiala
metadata - age categories
</commit_message>
<xml_diff>
--- a/supplementary_materials/TableS2_clinical_considerations.xlsx
+++ b/supplementary_materials/TableS2_clinical_considerations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Klara/2023holobiont/manuscript/supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B191082-1EB5-694D-96AB-D152B660791B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFF8795-E897-F94E-9C64-ABDE1DDE8387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33980" yWindow="2340" windowWidth="27640" windowHeight="16940" xr2:uid="{C2AB6BF0-9841-BE4E-A213-4C54AD9D1261}"/>
+    <workbookView xWindow="1260" yWindow="500" windowWidth="34580" windowHeight="21900" xr2:uid="{C2AB6BF0-9841-BE4E-A213-4C54AD9D1261}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,12 +155,6 @@
     <t>Clinical considerations</t>
   </si>
   <si>
-    <t>2019 HR Adult female - Admitted in Dec. 2018 due to head trauma (deep lesion) and treated with manuka honey and antibiotics. In June 2019 transferred to outside pool with recirculating seawater to fully recover prior to release. Sampled on day 321 (Oct. 2019) in rehabilitation.</t>
-  </si>
-  <si>
-    <t>2019 HR Subadult ND - Caught by trawling with small flipper lesion, otherwise healthy. Sampled on day 6 (May 2019) in rehabilitation. Released on day 12.</t>
-  </si>
-  <si>
     <t>2019 HR Adult female - Found floating with deep head wound and carapace lesion - deceased within 2 weeks of arrival to the centre. Sampled on day 1 of rehabilitation (June 2019).</t>
   </si>
   <si>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>2021 HR Adult male - Ventral skull fracture, treatment with antibiotics, struggled to dive and expell food remains at sampling date. Sampled on day 29 of rehabilitation (Aug. 2021).</t>
+  </si>
+  <si>
+    <t>2019 HR Juvenile ND - Caught by trawling with small flipper lesion, otherwise healthy. Sampled on day 6 (May 2019) in rehabilitation. Released on day 12.</t>
+  </si>
+  <si>
+    <t>2019 HR Subadult female - Admitted in Dec. 2018 due to head trauma (deep lesion) and treated with manuka honey and antibiotics. In June 2019 transferred to outside pool with recirculating seawater to fully recover prior to release. Sampled on day 321 (Oct. 2019) in rehabilitation.</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,7 +623,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -631,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -653,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -664,7 +664,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -675,7 +675,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -697,7 +697,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -741,7 +741,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -752,7 +752,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -763,7 +763,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -774,7 +774,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -785,7 +785,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -818,7 +818,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>